<commit_message>
Expediente Shannery 2 de mayo
</commit_message>
<xml_diff>
--- a/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
+++ b/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA EXPEDEDIENTES VIVOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972D96AC-B3D0-4784-BD27-3B874CEF274F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286BEFB3-BC41-47AA-B64E-01D100677D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSA" sheetId="11" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="MONICA PARDO" sheetId="8" r:id="rId9"/>
     <sheet name="RUBÉN MARTINEZ" sheetId="9" r:id="rId10"/>
     <sheet name="STEPHANI GUERRERO" sheetId="10" r:id="rId11"/>
+    <sheet name="SHANNERY CHAPARRO" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HSA!$A$1:$Q$37</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="353">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -1364,6 +1365,30 @@
 06/03/2025 ASESOR RECIBIÓ CORRECCION Y ESTA EN PROCESO DE REALIZAR LOS AJUSTES NECESARIOS
 28/02/2025 EN TRAMITE DE REVISIÒN Y CORRECCIÒN AUTO ALEGATOS
 21/02/2025 ASESOR INDICA QUE NO HAY NUEVOS ACTOS ADMINISTRATIVOS</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-008134</t>
+  </si>
+  <si>
+    <t>SOLICITUD DE REVOCATORIA DE MANDATO DEL ACTUAL ALCALDE DEL MUNICIPIO DE HONDA TOLIMA, SEÑOR JUAN ENRIQUE RONDON GARCIA</t>
+  </si>
+  <si>
+    <t>TOLIMA</t>
+  </si>
+  <si>
+    <t>HONDA</t>
+  </si>
+  <si>
+    <t>CARLOS HUGO MESA MAYNE</t>
+  </si>
+  <si>
+    <t>REVOCATORIA DE MANDATO</t>
+  </si>
+  <si>
+    <t>02/05/2025 ASIGNADO A LA ASESORA SHANNERY CHAPARRO</t>
+  </si>
+  <si>
+    <t>SHANNERY CHAPARRO</t>
   </si>
 </sst>
 </file>
@@ -1568,7 +1593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1656,6 +1681,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1964,12 +1992,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O62" sqref="O62"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37:Q37"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38:Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3958,6 +3986,57 @@
         <v>32</v>
       </c>
     </row>
+    <row r="38" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="14">
+        <v>45779</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="I38" s="14"/>
+      <c r="J38" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="K38" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" s="14">
+        <v>45779</v>
+      </c>
+      <c r="M38" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="N38" s="8">
+        <v>45779</v>
+      </c>
+      <c r="O38" s="14">
+        <v>45779</v>
+      </c>
+      <c r="P38" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q38" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:Q37" xr:uid="{868CBA12-E8F6-468A-9E1A-12215A2C5AF4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4425,6 +4504,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A65B1D2-9DDC-4748-A89D-A3B554A960BE}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="17" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="14">
+        <v>45779</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="14">
+        <v>45779</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="N2" s="8">
+        <v>45779</v>
+      </c>
+      <c r="O2" s="14">
+        <v>45779</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q4"/>

</xml_diff>

<commit_message>
Shannery expediente fecha caducidad
</commit_message>
<xml_diff>
--- a/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
+++ b/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA EXPEDEDIENTES VIVOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286BEFB3-BC41-47AA-B64E-01D100677D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1C4F97-11DD-4523-BCCE-8D60DFED0726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="353">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -1994,10 +1994,10 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O62" sqref="O62"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38:Q38"/>
+      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4011,7 +4011,9 @@
       <c r="H38" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="I38" s="14"/>
+      <c r="I38" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="J38" s="13" t="s">
         <v>351</v>
       </c>
@@ -4508,8 +4510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A65B1D2-9DDC-4748-A89D-A3B554A960BE}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4595,7 +4597,9 @@
       <c r="H2" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="I2" s="14"/>
+      <c r="I2" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="J2" s="13" t="s">
         <v>351</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion 12 de mayo de 2025
</commit_message>
<xml_diff>
--- a/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
+++ b/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA EXPEDEDIENTES VIVOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DD8DD0-0738-4B08-9948-2883BF2AB5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE97079-05B6-4892-B571-367FDA92B30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <sheet name="SHANNERY CHAPARRO" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HSA!$A$1:$Q$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HSA!$A$1:$Q$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="357">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -1397,6 +1397,18 @@
   <si>
     <t>05/05/2025 RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
   </si>
+  <si>
+    <t>CNE-E-DG-2025-008553</t>
+  </si>
+  <si>
+    <t>SOLICITUD DE INTERVENCIÓN POR VULNERACIÓN DE DERECHO DE REPLICA - ARTICULO 17 LEY 1909 DE 2018</t>
+  </si>
+  <si>
+    <t>DIEGO FABIAN CASTILLO QUINTERO</t>
+  </si>
+  <si>
+    <t>12/05/ 2025 RECIBIDO POR EL ASESOR</t>
+  </si>
 </sst>
 </file>
 
@@ -1405,7 +1417,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1448,6 +1460,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1600,7 +1618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1694,6 +1712,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2002,12 +2023,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O62" sqref="O62"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3042,310 +3063,310 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
+    <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>353</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" s="24">
+        <v>45782</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="24">
+        <v>45789</v>
+      </c>
+      <c r="M20" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="N20" s="7">
+        <v>45789</v>
+      </c>
+      <c r="O20" s="7">
+        <v>45789</v>
+      </c>
+      <c r="P20" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q20" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C21" s="8">
         <v>45246</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D21" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E21" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="F20" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="15" t="s">
+      <c r="F21" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H21" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I21" s="8">
         <v>45790</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J21" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K21" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L21" s="8">
         <v>45754</v>
       </c>
-      <c r="M20" s="15" t="s">
+      <c r="M21" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N21" s="7">
         <v>45775</v>
       </c>
-      <c r="O20" s="8">
+      <c r="O21" s="8">
         <v>45691</v>
       </c>
-      <c r="P20" s="15" t="s">
+      <c r="P21" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="Q20" s="15" t="s">
+      <c r="Q21" s="15" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+    <row r="22" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C22" s="26">
         <v>45264</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D22" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E22" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F22" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G22" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H22" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="I21" s="26">
+      <c r="I22" s="26">
         <v>46315</v>
       </c>
-      <c r="J21" s="27" t="s">
+      <c r="J22" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="K21" s="25" t="s">
+      <c r="K22" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="L21" s="26">
+      <c r="L22" s="26">
         <v>45735</v>
       </c>
-      <c r="M21" s="27" t="s">
+      <c r="M22" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N22" s="11">
         <v>45771</v>
       </c>
-      <c r="O21" s="26">
+      <c r="O22" s="26">
         <v>45691</v>
       </c>
-      <c r="P21" s="27" t="s">
+      <c r="P22" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="Q21" s="27" t="s">
+      <c r="Q22" s="27" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+    <row r="23" spans="1:17" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C23" s="28">
         <v>45653</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D23" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E23" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F23" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G23" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H23" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I23" s="28">
         <v>46549</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J23" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="K22" s="10" t="s">
+      <c r="K23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L22" s="28">
+      <c r="L23" s="28">
         <v>45712</v>
       </c>
-      <c r="M22" s="10" t="s">
+      <c r="M23" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N23" s="11">
         <v>45751</v>
-      </c>
-      <c r="O22" s="8">
-        <v>45691</v>
-      </c>
-      <c r="P22" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q22" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="11">
-        <v>45541</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="I23" s="11">
-        <v>46636</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L23" s="11">
-        <v>45705</v>
-      </c>
-      <c r="M23" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="N23" s="11">
-        <v>45762</v>
       </c>
       <c r="O23" s="8">
         <v>45691</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="P23" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="Q23" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="B24" s="15" t="s">
+      <c r="Q23" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="8">
-        <v>45466</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="I24" s="8">
-        <v>45466</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="K24" s="15" t="s">
+      <c r="C24" s="11">
+        <v>45541</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="I24" s="11">
+        <v>46636</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="K24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L24" s="8">
-        <v>45673</v>
-      </c>
-      <c r="M24" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="N24" s="7">
-        <v>45755</v>
+      <c r="L24" s="11">
+        <v>45705</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="N24" s="11">
+        <v>45762</v>
       </c>
       <c r="O24" s="8">
         <v>45691</v>
       </c>
-      <c r="P24" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="Q24" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="B25" s="10" t="s">
+      <c r="P24" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="28">
-        <v>45665</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="I25" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="L25" s="28">
-        <v>45700</v>
-      </c>
-      <c r="M25" s="10" t="s">
-        <v>257</v>
+      <c r="C25" s="8">
+        <v>45466</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="I25" s="8">
+        <v>45466</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" s="8">
+        <v>45673</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>247</v>
       </c>
       <c r="N25" s="7">
         <v>45755</v>
@@ -3353,211 +3374,211 @@
       <c r="O25" s="8">
         <v>45691</v>
       </c>
-      <c r="P25" s="10" t="s">
+      <c r="P25" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="Q25" s="10" t="s">
+      <c r="Q25" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>196</v>
+        <v>18</v>
       </c>
       <c r="C26" s="28">
-        <v>45758</v>
+        <v>45665</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>36</v>
+        <v>253</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="I26" s="28" t="s">
         <v>36</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="L26" s="28">
-        <v>45758</v>
+        <v>45700</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="N26" s="7">
-        <v>45771</v>
+        <v>45755</v>
       </c>
       <c r="O26" s="8">
-        <v>45775</v>
-      </c>
-      <c r="P26" s="15" t="s">
-        <v>264</v>
+        <v>45691</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>249</v>
       </c>
       <c r="Q26" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="8">
-        <v>45505</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="I27" s="8">
-        <v>46395</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="K27" s="15" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" s="28">
+        <v>45758</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="K27" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L27" s="8">
-        <v>45720</v>
-      </c>
-      <c r="M27" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="N27" s="8">
+      <c r="L27" s="28">
+        <v>45758</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="N27" s="7">
         <v>45771</v>
       </c>
       <c r="O27" s="8">
-        <v>45691</v>
+        <v>45775</v>
       </c>
       <c r="P27" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="Q27" s="15" t="s">
+      <c r="Q27" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>273</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>274</v>
+        <v>265</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="C28" s="8">
-        <v>43999</v>
+        <v>45505</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>37</v>
+        <v>269</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>111</v>
+        <v>270</v>
       </c>
       <c r="I28" s="8">
-        <v>44967</v>
+        <v>46395</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="L28" s="8">
-        <v>45615</v>
+        <v>45720</v>
       </c>
       <c r="M28" s="15" t="s">
-        <v>328</v>
-      </c>
-      <c r="N28" s="8" t="s">
-        <v>329</v>
+        <v>272</v>
+      </c>
+      <c r="N28" s="8">
+        <v>45771</v>
       </c>
       <c r="O28" s="8">
         <v>45691</v>
       </c>
       <c r="P28" s="15" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="Q28" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>282</v>
+    <row r="29" spans="1:17" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>273</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="7">
-        <v>45266</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H29" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C29" s="8">
+        <v>43999</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="I29" s="7">
-        <v>46232</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L29" s="7">
-        <v>45693</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>330</v>
+      <c r="I29" s="8">
+        <v>44967</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" s="8">
+        <v>45615</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>328</v>
       </c>
       <c r="N29" s="8" t="s">
         <v>329</v>
@@ -3565,52 +3586,52 @@
       <c r="O29" s="8">
         <v>45691</v>
       </c>
-      <c r="P29" s="6" t="s">
+      <c r="P29" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="Q29" s="6" t="s">
+      <c r="Q29" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="8">
-        <v>44861</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="I30" s="8">
-        <v>45790</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>289</v>
-      </c>
-      <c r="K30" s="15" t="s">
+      <c r="C30" s="7">
+        <v>45266</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I30" s="7">
+        <v>46232</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="K30" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L30" s="8">
-        <v>45720</v>
-      </c>
-      <c r="M30" s="15" t="s">
-        <v>331</v>
+      <c r="L30" s="7">
+        <v>45693</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>330</v>
       </c>
       <c r="N30" s="8" t="s">
         <v>329</v>
@@ -3618,16 +3639,16 @@
       <c r="O30" s="8">
         <v>45691</v>
       </c>
-      <c r="P30" s="15" t="s">
+      <c r="P30" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="Q30" s="15" t="s">
+      <c r="Q30" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>18</v>
@@ -3636,10 +3657,10 @@
         <v>44861</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>34</v>
+        <v>288</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>268</v>
+        <v>36</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>36</v>
@@ -3648,75 +3669,75 @@
         <v>37</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="I31" s="8">
-        <v>45729</v>
+        <v>45790</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="L31" s="8">
-        <v>45748</v>
+        <v>45720</v>
       </c>
       <c r="M31" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="N31" s="8">
-        <v>45775</v>
+        <v>331</v>
+      </c>
+      <c r="N31" s="8" t="s">
+        <v>329</v>
       </c>
       <c r="O31" s="8">
         <v>45691</v>
       </c>
       <c r="P31" s="15" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="Q31" s="15" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="102" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B32" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="7">
-        <v>45440</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="I32" s="7">
-        <v>46535</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L32" s="7">
-        <v>45714</v>
-      </c>
-      <c r="M32" s="6" t="s">
-        <v>311</v>
+      <c r="C32" s="8">
+        <v>44861</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="8">
+        <v>45729</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L32" s="8">
+        <v>45748</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>300</v>
       </c>
       <c r="N32" s="8">
         <v>45775</v>
@@ -3724,58 +3745,58 @@
       <c r="O32" s="8">
         <v>45691</v>
       </c>
-      <c r="P32" s="6" t="s">
+      <c r="P32" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="Q32" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="Q32" s="15" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="7">
-        <v>45715</v>
+        <v>45440</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>24</v>
+        <v>309</v>
       </c>
       <c r="I33" s="7">
-        <v>46992</v>
+        <v>46535</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="K33" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L33" s="7">
-        <v>45720</v>
+        <v>45714</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="N33" s="8">
         <v>45775</v>
       </c>
       <c r="O33" s="8">
-        <v>45715</v>
+        <v>45691</v>
       </c>
       <c r="P33" s="6" t="s">
         <v>301</v>
@@ -3785,272 +3806,325 @@
       </c>
     </row>
     <row r="34" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="B34" s="9" t="s">
+      <c r="A34" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="11">
-        <v>45709</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="H34" s="9" t="s">
+      <c r="C34" s="7">
+        <v>45715</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I34" s="11">
-        <v>46804</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="K34" s="9" t="s">
+      <c r="I34" s="7">
+        <v>46992</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="K34" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L34" s="11">
-        <v>45735</v>
-      </c>
-      <c r="M34" s="9" t="s">
-        <v>325</v>
+      <c r="L34" s="7">
+        <v>45720</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>318</v>
       </c>
       <c r="N34" s="8">
-        <v>45762</v>
+        <v>45775</v>
       </c>
       <c r="O34" s="8">
-        <v>45713</v>
+        <v>45715</v>
       </c>
       <c r="P34" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="Q34" s="9" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="Q34" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>347</v>
+        <v>319</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C35" s="11">
-        <v>45417</v>
+        <v>45709</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>35</v>
+        <v>171</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="G35" s="32" t="s">
-        <v>350</v>
+        <v>322</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>323</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="I35" s="11">
+        <v>46804</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>352</v>
+        <v>324</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L35" s="11">
-        <v>45782</v>
+        <v>45735</v>
       </c>
       <c r="M35" s="9" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="N35" s="8">
-        <v>45783</v>
+        <v>45762</v>
       </c>
       <c r="O35" s="8">
-        <v>45714</v>
+        <v>45713</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>301</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>32</v>
+        <v>327</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C36" s="11">
-        <v>45776</v>
+        <v>45417</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>334</v>
+        <v>35</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="G36" s="30" t="s">
-        <v>335</v>
+        <v>349</v>
+      </c>
+      <c r="G36" s="32" t="s">
+        <v>350</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>199</v>
+        <v>351</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>36</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>336</v>
+        <v>352</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L36" s="11">
-        <v>45776</v>
+        <v>45782</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="N36" s="11">
-        <v>45776</v>
-      </c>
-      <c r="O36" s="11">
+        <v>352</v>
+      </c>
+      <c r="N36" s="8">
+        <v>45783</v>
+      </c>
+      <c r="O36" s="8">
         <v>45714</v>
       </c>
-      <c r="P36" s="9" t="s">
+      <c r="P36" s="6" t="s">
         <v>301</v>
       </c>
       <c r="Q36" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
+    <row r="37" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="11">
+        <v>45776</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>335</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L37" s="11">
+        <v>45776</v>
+      </c>
+      <c r="M37" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="N37" s="11">
+        <v>45776</v>
+      </c>
+      <c r="O37" s="11">
+        <v>45714</v>
+      </c>
+      <c r="P37" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q37" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B38" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C38" s="14">
         <v>45700</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D38" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E38" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F38" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G38" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H38" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I37" s="14">
+      <c r="I38" s="14">
         <v>46795</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J38" s="13" t="s">
         <v>296</v>
-      </c>
-      <c r="K37" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L37" s="14">
-        <v>45744</v>
-      </c>
-      <c r="M37" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="N37" s="8">
-        <v>45777</v>
-      </c>
-      <c r="O37" s="14">
-        <v>45701</v>
-      </c>
-      <c r="P37" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q37" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="14">
-        <v>45779</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>345</v>
       </c>
       <c r="K38" s="13" t="s">
         <v>26</v>
       </c>
       <c r="L38" s="14">
+        <v>45744</v>
+      </c>
+      <c r="M38" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="N38" s="8">
+        <v>45777</v>
+      </c>
+      <c r="O38" s="14">
+        <v>45701</v>
+      </c>
+      <c r="P38" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q38" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="14">
         <v>45779</v>
       </c>
-      <c r="M38" s="13" t="s">
+      <c r="D39" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J39" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="N38" s="8">
+      <c r="K39" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" s="14">
         <v>45779</v>
       </c>
-      <c r="O38" s="14">
+      <c r="M39" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="N39" s="8">
         <v>45779</v>
       </c>
-      <c r="P38" s="13" t="s">
+      <c r="O39" s="14">
+        <v>45779</v>
+      </c>
+      <c r="P39" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="Q38" s="31" t="s">
+      <c r="Q39" s="31" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q37" xr:uid="{868CBA12-E8F6-468A-9E1A-12215A2C5AF4}"/>
+  <autoFilter ref="A1:Q38" xr:uid="{868CBA12-E8F6-468A-9E1A-12215A2C5AF4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -5491,10 +5565,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5976,6 +6050,59 @@
         <v>144</v>
       </c>
       <c r="Q9" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="48" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>353</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="24">
+        <v>45782</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="K10" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="24">
+        <v>45789</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="N10" s="7">
+        <v>45789</v>
+      </c>
+      <c r="O10" s="7">
+        <v>45789</v>
+      </c>
+      <c r="P10" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q10" s="23" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualizacion 19 de mayo
</commit_message>
<xml_diff>
--- a/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
+++ b/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA EXPEDEDIENTES VIVOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3F2E2F-1707-40D7-A1F9-450563B87BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DA1E72-7871-4E14-B660-E827DBEF5EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSA" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="298">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -651,56 +651,7 @@
     <t>INPUGNACIONES</t>
   </si>
   <si>
-    <t>16/01/2025- AUTO N° 006 DE 2025- CORRE TRASLADO DE PRUEBAS
-29/08/2024: AUTO NO 109 DEL 13-08/2024 PRUEBAS DE IMPUGNACIÓN.
-01/02/2024  SE PROFIRIO AUTO NO 006 REITERANDO DECRETO DE PRUEBAS; 
-SE RECIBIERON HASTA EL 25 DE ABRIL DEL AÑO EN CURSO SOPORTES DE COMUNICACIÓN. SE PROFIRIÓ. AUTO N 109 DEL 13 DE AGOSTO DE 2024, EL CUAL DECRETÓ LA PRÁCTICA DE UNAS PRUEBAS PARA MEJOR PROVEER. SE NOTIFICÓ EL 28 DE AGOSTO DE 2024. SE PROFIRIÓ ACTO ADMINISTRATIVO NO 127 DEL 23 DE OCTUBRE DE 2024, A TRAVÉS DEL CUAL SE INSTA AL MOVIMIENTO COLOMBIA HUMANA A DAR CUMPLIMIENTO A LO CONMINADO EN EL ARTÍCULO PRIMERO DEL AUTO 109.</t>
-  </si>
-  <si>
-    <t>08/04/2025 PENDIENTE RESOLUCIÓN PARA SER FIRMADA Y PENDIENTE DE NOTIFICACIONES
-06/03/2025 - ENVIADA A RADICAR POR MONICA RESOLUCIÓN QUE CONCEDE IMPUGNACIÓN
-28/02/2025 RESOLUCIÓN CONCEDIENDO IMPUGNACIÓN, ENVIADA A REVISIÓN DE MIGUEL EL 27 DE FEBRERO DE 2025
-AUTO COMUNICADO EL 16 DE ENERO DE 2025, TÉRMINOS CUMPLIDOS EL 24 DE ENERO D 2025, EN PROYECCIÓN DECISIÓN
-16/01/2025 YA LLEGARON LAS NOTIFICACIONES
-15/01/2025 SE DEBE CORRER TRASLADO</t>
-  </si>
-  <si>
     <t>LAURA ORTEGON</t>
-  </si>
-  <si>
-    <t>CNE-E-DG-2025-000141</t>
-  </si>
-  <si>
-    <t>SOLICITUD DE REVOCATORIA DE INSCRIPCIÓN DEL CANDIDATO A LA GOBERNACIÓN DE PUTUMAYO, EL SEÑOR JOHN GABRIEL MOLINA ACOSTA, PARA LAS ELECCIONES ATIPICAS DEL 2025</t>
-  </si>
-  <si>
-    <t>PUTUMAYO</t>
-  </si>
-  <si>
-    <t>LUIS ALFONSO CABRERA</t>
-  </si>
-  <si>
-    <t>REVOCATORIA</t>
-  </si>
-  <si>
-    <t>19/02/2025 SE EXPIDIO OFICIO 053 RESPECTO A RESPUESTA A ACCIÓN DE TUTELA
-12/02/2025 - RESOLUCIÓN No 00554 ESTARSE A LO RESUELTO EN LAS RESOLUCIONES No 00267 y 00479  DE 2025 QUE DECIDIERON NO REVOCAR LA INSCRIPCIÓN DE LA CANDIDATURA  A LA GOGERNACIÓN DE JHON GABRIEL MOLINA ACOSTA - NOTIFICADA EN AUDIENCIA DEL 12/02/2025
- 06/02/2025 - RESOLUCIÓN 00479 POR MEDIO DE LA CUAL NO SE REPONE LA RESOLUCIÓN 00262 DEL 29 DE ENERO DE 2025 
-29/01/2025 - RESOLUCIÓN No 0262 - NO SE REVOCA LA INSCRIPCIÓN DEL CANDIDATO A LA GOBERNACIÓN DE PUTUMAYO,  JOHN GABRIEL MOLINA ACOSTA, PARA LAS ELECCIONES ATIPICAS DEL 2025
-15/01/2025- AUTO 009- CORRE TRASLADO DE PRUEBAS
-10/01/2025- AUTO NO 002- CORRIGE AUTO 001 Y COMUNICA A LAS AGRUPACIONES POLÍTICAS AICO, MAIZ Y PARTIDO CONSERVADOR
-08/01/2025 AUTO NO. 001 DEL 8 DE ENERO DE 2025 AVOCA CONOCIMIENTO Y SOLICITA PRUEBA</t>
-  </si>
-  <si>
-    <t>08/04/2025 PENDIENTE PARA ARCHIVO
-06/03/2025 - PENDIENTE DE ARCHIVO  ENTREGA A LUISA CUCHIBAQUE 
-28/02/2025 SIGUE EN ESPERA DE OFICIO 053 RESPECTO A RESPUESTA A ACCIÓN DE TUTELA
-19/02/2025 SE EXPIDIO OFICIO 053 RESPECTO A RESPUESTA A ACCIÓN DE TUTELA
-12/02/2025 NOTIFICADA EN AUDIENCIA
-06/02/2025 PENDIENTE DE DECIDIR RESOLUCIÓN DE ATENERSE A LO RESUELTO 
-SE RECIBIÓ RECURSO DE REPOSICIÓN EL DÍA 30 DE ENERO DE 2025, ACTUALMENTE SE ESTÁ RESOLVIENDO RECURSO
-23/01/2025 CORRIENDO TERMINOS
-CORRIENDO TÉRMINOS Y EN ESPERA DE COMUNICACIONES</t>
   </si>
   <si>
     <t>CNE-E-DG-2025-006989</t>
@@ -1248,6 +1199,22 @@
   <si>
     <t>15/05/2025 AUTO N° 046 AVOCA CONOCIMIENTO
 12/05/ 2025 RECIBIDO POR EL ASESOR</t>
+  </si>
+  <si>
+    <t>01/04/2025 REOSLUCION 01459 QUE CONCEDE IMPUGNACION
+16/01/2025- AUTO N° 006 DE 2025- CORRE TRASLADO DE PRUEBAS
+29/08/2024: AUTO NO 109 DEL 13-08/2024 PRUEBAS DE IMPUGNACIÓN.
+01/02/2024  SE PROFIRIO AUTO NO 006 REITERANDO DECRETO DE PRUEBAS; 
+SE RECIBIERON HASTA EL 25 DE ABRIL DEL AÑO EN CURSO SOPORTES DE COMUNICACIÓN. SE PROFIRIÓ. AUTO N 109 DEL 13 DE AGOSTO DE 2024, EL CUAL DECRETÓ LA PRÁCTICA DE UNAS PRUEBAS PARA MEJOR PROVEER. SE NOTIFICÓ EL 28 DE AGOSTO DE 2024. SE PROFIRIÓ ACTO ADMINISTRATIVO NO 127 DEL 23 DE OCTUBRE DE 2024, A TRAVÉS DEL CUAL SE INSTA AL MOVIMIENTO COLOMBIA HUMANA A DAR CUMPLIMIENTO A LO CONMINADO EN EL ARTÍCULO PRIMERO DEL AUTO 109.</t>
+  </si>
+  <si>
+    <t>06/05/2025 RECIBIDA CONSTANCIA DE NOTIFICACION DE LA REOSLUCION 01459 QUE CONCEDE IMPUGNACION
+08/04/2025 PENDIENTE RESOLUCIÓN PARA SER FIRMADA Y PENDIENTE DE NOTIFICACIONES
+06/03/2025 - ENVIADA A RADICAR POR MONICA RESOLUCIÓN QUE CONCEDE IMPUGNACIÓN
+28/02/2025 RESOLUCIÓN CONCEDIENDO IMPUGNACIÓN, ENVIADA A REVISIÓN DE MIGUEL EL 27 DE FEBRERO DE 2025
+AUTO COMUNICADO EL 16 DE ENERO DE 2025, TÉRMINOS CUMPLIDOS EL 24 DE ENERO D 2025, EN PROYECCIÓN DECISIÓN
+16/01/2025 YA LLEGARON LAS NOTIFICACIONES
+15/01/2025 SE DEBE CORRER TRASLADO</t>
   </si>
 </sst>
 </file>
@@ -1849,10 +1816,10 @@
   </sheetPr>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O62" sqref="O62"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:Q39"/>
+      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1962,7 +1929,7 @@
         <v>46164</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>25</v>
@@ -1971,7 +1938,7 @@
         <v>45761</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="N2" s="8">
         <v>45791</v>
@@ -2024,7 +1991,7 @@
         <v>45735</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="N3" s="8">
         <v>45761</v>
@@ -2077,7 +2044,7 @@
         <v>45722</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="N4" s="7">
         <v>45792</v>
@@ -2089,7 +2056,7 @@
         <v>49</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -2130,7 +2097,7 @@
         <v>45705</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="N5" s="11">
         <v>45792</v>
@@ -2142,7 +2109,7 @@
         <v>49</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="127.5" x14ac:dyDescent="0.2">
@@ -2183,7 +2150,7 @@
         <v>45708</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="N6" s="11">
         <v>45792</v>
@@ -2195,12 +2162,12 @@
         <v>49</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>35</v>
@@ -2209,7 +2176,7 @@
         <v>45791</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>148</v>
@@ -2218,7 +2185,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>39</v>
@@ -2227,7 +2194,7 @@
         <v>31</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>25</v>
@@ -2236,7 +2203,7 @@
         <v>45792</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="N7" s="11">
         <v>45792</v>
@@ -2395,7 +2362,7 @@
         <v>45698</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="N10" s="7">
         <v>45793</v>
@@ -2448,7 +2415,7 @@
         <v>45744</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="N11" s="7">
         <v>45793</v>
@@ -2501,7 +2468,7 @@
         <v>45714</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="N12" s="7">
         <v>45793</v>
@@ -2554,7 +2521,7 @@
         <v>45734</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="N13" s="7">
         <v>45793</v>
@@ -2607,7 +2574,7 @@
         <v>45771</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="N14" s="7">
         <v>45793</v>
@@ -2660,7 +2627,7 @@
         <v>45748</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="N15" s="7">
         <v>45793</v>
@@ -2713,7 +2680,7 @@
         <v>45735</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="N16" s="7">
         <v>45793</v>
@@ -2766,7 +2733,7 @@
         <v>45769</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="N17" s="7">
         <v>45793</v>
@@ -2783,7 +2750,7 @@
     </row>
     <row r="18" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>141</v>
@@ -2792,7 +2759,7 @@
         <v>45782</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>31</v>
@@ -2801,16 +2768,16 @@
         <v>31</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="I18" s="23" t="s">
         <v>31</v>
       </c>
       <c r="J18" s="22" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="K18" s="24" t="s">
         <v>25</v>
@@ -2819,7 +2786,7 @@
         <v>45792</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="N18" s="7">
         <v>45792</v>
@@ -2925,7 +2892,7 @@
         <v>45735</v>
       </c>
       <c r="M20" s="26" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="N20" s="11">
         <v>45792</v>
@@ -2934,10 +2901,10 @@
         <v>45691</v>
       </c>
       <c r="P20" s="26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q20" s="26" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="140.25" x14ac:dyDescent="0.2">
@@ -2978,7 +2945,7 @@
         <v>45712</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="N21" s="11">
         <v>45792</v>
@@ -2987,13 +2954,13 @@
         <v>45691</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q21" s="26" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>173</v>
       </c>
@@ -3022,281 +2989,281 @@
         <v>45466</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>178</v>
+        <v>296</v>
       </c>
       <c r="K22" s="15" t="s">
         <v>25</v>
       </c>
       <c r="L22" s="8">
-        <v>45673</v>
+        <v>45748</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>179</v>
+        <v>297</v>
       </c>
       <c r="N22" s="7">
-        <v>45755</v>
+        <v>45783</v>
       </c>
       <c r="O22" s="8">
         <v>45691</v>
       </c>
       <c r="P22" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q22" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="11">
+        <v>45684</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="11">
+        <v>46779</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="11">
+        <v>45735</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="N23" s="8">
+        <v>45792</v>
+      </c>
+      <c r="O23" s="8">
+        <v>45688</v>
+      </c>
+      <c r="P23" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q23" s="26" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="27">
+        <v>45758</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="H24" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="27">
+        <v>45758</v>
+      </c>
+      <c r="M24" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="N24" s="7">
+        <v>45771</v>
+      </c>
+      <c r="O24" s="8">
+        <v>45775</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="27">
-        <v>45665</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="H23" s="10" t="s">
+      <c r="C25" s="8">
+        <v>45505</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="I25" s="8">
+        <v>46395</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="8">
+        <v>45720</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="N25" s="8">
+        <v>45771</v>
+      </c>
+      <c r="O25" s="8">
+        <v>45691</v>
+      </c>
+      <c r="P25" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="I23" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="K23" s="10" t="s">
+      <c r="Q25" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" s="8">
+        <v>43999</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" s="8">
+        <v>44967</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="K26" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="L23" s="27">
-        <v>45700</v>
-      </c>
-      <c r="M23" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="N23" s="7">
-        <v>45755</v>
-      </c>
-      <c r="O23" s="8">
-        <v>45691</v>
-      </c>
-      <c r="P23" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q23" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="11">
-        <v>45684</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24" s="11">
-        <v>46779</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24" s="11">
-        <v>45735</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="N24" s="8">
-        <v>45792</v>
-      </c>
-      <c r="O24" s="8">
-        <v>45688</v>
-      </c>
-      <c r="P24" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q24" s="26" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C25" s="27">
-        <v>45758</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="I25" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L25" s="27">
-        <v>45758</v>
-      </c>
-      <c r="M25" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="N25" s="7">
-        <v>45771</v>
-      </c>
-      <c r="O25" s="8">
-        <v>45775</v>
-      </c>
-      <c r="P25" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q25" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="8">
-        <v>45505</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="I26" s="8">
-        <v>46395</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="K26" s="15" t="s">
-        <v>25</v>
-      </c>
       <c r="L26" s="8">
-        <v>45720</v>
+        <v>45615</v>
       </c>
       <c r="M26" s="15" t="s">
-        <v>202</v>
+        <v>263</v>
       </c>
       <c r="N26" s="8">
-        <v>45771</v>
+        <v>45791</v>
       </c>
       <c r="O26" s="8">
         <v>45691</v>
       </c>
       <c r="P26" s="15" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="Q26" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>203</v>
+    <row r="27" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>200</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C27" s="8">
-        <v>43999</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H27" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="7">
+        <v>45266</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I27" s="8">
-        <v>44967</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="K27" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="L27" s="8">
-        <v>45615</v>
-      </c>
-      <c r="M27" s="15" t="s">
-        <v>272</v>
+      <c r="I27" s="7">
+        <v>46232</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="7">
+        <v>45693</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>264</v>
       </c>
       <c r="N27" s="8">
         <v>45791</v>
@@ -3304,308 +3271,308 @@
       <c r="O27" s="8">
         <v>45691</v>
       </c>
-      <c r="P27" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q27" s="15" t="s">
+      <c r="P27" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q27" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="7">
-        <v>45266</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I28" s="7">
-        <v>46232</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L28" s="7">
-        <v>45693</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>273</v>
+      <c r="C28" s="8">
+        <v>44861</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="8">
+        <v>45790</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" s="8">
+        <v>45720</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>265</v>
       </c>
       <c r="N28" s="8">
-        <v>45791</v>
+        <v>45761</v>
       </c>
       <c r="O28" s="8">
         <v>45691</v>
       </c>
-      <c r="P28" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q28" s="6" t="s">
+      <c r="P28" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q28" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B29" s="15" t="s">
+    <row r="29" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="8">
-        <v>44861</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="8">
-        <v>45790</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="L29" s="8">
-        <v>45720</v>
-      </c>
-      <c r="M29" s="15" t="s">
-        <v>274</v>
+      <c r="C29" s="7">
+        <v>45440</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="I29" s="7">
+        <v>46535</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L29" s="7">
+        <v>45714</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>221</v>
       </c>
       <c r="N29" s="8">
-        <v>45761</v>
+        <v>45775</v>
       </c>
       <c r="O29" s="8">
         <v>45691</v>
       </c>
-      <c r="P29" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q29" s="15" t="s">
+      <c r="P29" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q29" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="7">
-        <v>45440</v>
+        <v>45715</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="F30" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>227</v>
-      </c>
       <c r="H30" s="6" t="s">
-        <v>228</v>
+        <v>23</v>
       </c>
       <c r="I30" s="7">
-        <v>46535</v>
+        <v>46992</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>229</v>
+        <v>285</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L30" s="7">
-        <v>45714</v>
+        <v>45784</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>230</v>
+        <v>286</v>
       </c>
       <c r="N30" s="8">
-        <v>45775</v>
+        <v>45793</v>
       </c>
       <c r="O30" s="8">
-        <v>45691</v>
+        <v>45715</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="102" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="11">
+        <v>45709</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="11">
+        <v>46804</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="7">
-        <v>45715</v>
-      </c>
-      <c r="D31" s="6" t="s">
+      <c r="K31" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31" s="11">
+        <v>45735</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="N31" s="8">
+        <v>45761</v>
+      </c>
+      <c r="O31" s="8">
+        <v>45713</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q31" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" s="7">
-        <v>46992</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L31" s="7">
-        <v>45784</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="N31" s="8">
-        <v>45793</v>
-      </c>
-      <c r="O31" s="8">
-        <v>45715</v>
-      </c>
-      <c r="P31" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q31" s="6" t="s">
+    </row>
+    <row r="32" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="11">
+        <v>45417</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="G32" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="11">
+        <v>45786</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="N32" s="8">
+        <v>45791</v>
+      </c>
+      <c r="O32" s="8">
+        <v>45714</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q32" s="9" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="11">
-        <v>45709</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="11">
-        <v>46804</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="L32" s="11">
-        <v>45735</v>
-      </c>
-      <c r="M32" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="N32" s="8">
-        <v>45761</v>
-      </c>
-      <c r="O32" s="8">
-        <v>45713</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q32" s="9" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="11">
-        <v>45417</v>
+        <v>45776</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>30</v>
+        <v>235</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="G33" s="31" t="s">
-        <v>259</v>
+        <v>235</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>236</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>260</v>
+        <v>144</v>
       </c>
       <c r="I33" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>25</v>
@@ -3614,16 +3581,16 @@
         <v>45786</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="N33" s="8">
+        <v>262</v>
+      </c>
+      <c r="N33" s="11">
         <v>45791</v>
       </c>
-      <c r="O33" s="8">
+      <c r="O33" s="11">
         <v>45714</v>
       </c>
-      <c r="P33" s="6" t="s">
-        <v>222</v>
+      <c r="P33" s="9" t="s">
+        <v>213</v>
       </c>
       <c r="Q33" s="9" t="s">
         <v>28</v>
@@ -3631,149 +3598,149 @@
     </row>
     <row r="34" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="B34" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="11">
-        <v>45776</v>
+        <v>45758</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>243</v>
+        <v>37</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>245</v>
+        <v>31</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="I34" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J34" s="9" t="s">
-        <v>270</v>
+      <c r="J34" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L34" s="11">
-        <v>45786</v>
+      <c r="L34" s="7">
+        <v>45775</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="N34" s="11">
-        <v>45791</v>
-      </c>
-      <c r="O34" s="11">
-        <v>45714</v>
+        <v>277</v>
+      </c>
+      <c r="N34" s="8">
+        <v>45792</v>
+      </c>
+      <c r="O34" s="8">
+        <v>45775</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="11">
-        <v>45758</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K35" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="7">
+        <v>45638</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="7">
+        <v>46733</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L35" s="7">
-        <v>45775</v>
-      </c>
-      <c r="M35" s="9" t="s">
-        <v>286</v>
+        <v>45748</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>279</v>
       </c>
       <c r="N35" s="8">
         <v>45792</v>
       </c>
       <c r="O35" s="8">
-        <v>45775</v>
+        <v>45691</v>
       </c>
       <c r="P35" s="9" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="165.75" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="7">
-        <v>45638</v>
+        <v>45161</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="I36" s="7">
-        <v>46733</v>
+        <v>46257</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K36" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K36" s="9" t="s">
         <v>25</v>
       </c>
       <c r="L36" s="7">
-        <v>45748</v>
+        <v>45370</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>288</v>
+        <v>96</v>
       </c>
       <c r="N36" s="8">
         <v>45792</v>
@@ -3782,121 +3749,121 @@
         <v>45691</v>
       </c>
       <c r="P36" s="9" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B37" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="7">
-        <v>45161</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I37" s="7">
-        <v>46257</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="K37" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="L37" s="7">
-        <v>45370</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>96</v>
+      <c r="C37" s="14">
+        <v>45700</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="I37" s="14">
+        <v>46795</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37" s="14">
+        <v>45744</v>
+      </c>
+      <c r="M37" s="13" t="s">
+        <v>238</v>
       </c>
       <c r="N37" s="8">
-        <v>45792</v>
-      </c>
-      <c r="O37" s="8">
-        <v>45691</v>
-      </c>
-      <c r="P37" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q37" s="9" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
+        <v>45777</v>
+      </c>
+      <c r="O37" s="14">
+        <v>45701</v>
+      </c>
+      <c r="P37" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q37" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="14">
+        <v>45779</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="K38" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L38" s="14">
+        <v>45779</v>
+      </c>
+      <c r="M38" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="N38" s="8">
+        <v>45779</v>
+      </c>
+      <c r="O38" s="14">
+        <v>45779</v>
+      </c>
+      <c r="P38" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="B38" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="14">
-        <v>45700</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="I38" s="14">
-        <v>46795</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L38" s="14">
-        <v>45744</v>
-      </c>
-      <c r="M38" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="N38" s="8">
-        <v>45777</v>
-      </c>
-      <c r="O38" s="14">
-        <v>45701</v>
-      </c>
-      <c r="P38" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q38" s="13" t="s">
+      <c r="Q38" s="30" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>35</v>
@@ -3905,25 +3872,25 @@
         <v>45779</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="I39" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="K39" s="13" t="s">
         <v>25</v>
@@ -3932,7 +3899,7 @@
         <v>45779</v>
       </c>
       <c r="M39" s="13" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="N39" s="8">
         <v>45779</v>
@@ -3941,7 +3908,7 @@
         <v>45779</v>
       </c>
       <c r="P39" s="13" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="Q39" s="30" t="s">
         <v>28</v>
@@ -4022,7 +3989,7 @@
     </row>
     <row r="2" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>18</v>
@@ -4031,25 +3998,25 @@
         <v>45440</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="I2" s="7">
         <v>46535</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>25</v>
@@ -4058,7 +4025,7 @@
         <v>45714</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="N2" s="8">
         <v>45775</v>
@@ -4067,7 +4034,7 @@
         <v>45691</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>28</v>
@@ -4075,7 +4042,7 @@
     </row>
     <row r="3" spans="1:17" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>18</v>
@@ -4084,16 +4051,16 @@
         <v>45715</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>23</v>
@@ -4102,7 +4069,7 @@
         <v>46992</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>25</v>
@@ -4111,7 +4078,7 @@
         <v>45784</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="N3" s="8">
         <v>45793</v>
@@ -4120,7 +4087,7 @@
         <v>45715</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>28</v>
@@ -4128,7 +4095,7 @@
     </row>
     <row r="4" spans="1:17" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>18</v>
@@ -4137,16 +4104,16 @@
         <v>45709</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>23</v>
@@ -4155,7 +4122,7 @@
         <v>46804</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>25</v>
@@ -4164,7 +4131,7 @@
         <v>45735</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="N4" s="8">
         <v>45761</v>
@@ -4173,15 +4140,15 @@
         <v>45713</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>35</v>
@@ -4190,25 +4157,25 @@
         <v>45417</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>30</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="G5" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>259</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>268</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>25</v>
@@ -4217,7 +4184,7 @@
         <v>45786</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="N5" s="8">
         <v>45791</v>
@@ -4226,7 +4193,7 @@
         <v>45714</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q5" s="9" t="s">
         <v>28</v>
@@ -4234,7 +4201,7 @@
     </row>
     <row r="6" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>35</v>
@@ -4243,16 +4210,16 @@
         <v>45776</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>144</v>
@@ -4261,7 +4228,7 @@
         <v>31</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>25</v>
@@ -4270,7 +4237,7 @@
         <v>45786</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="N6" s="11">
         <v>45791</v>
@@ -4279,7 +4246,7 @@
         <v>45714</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q6" s="9" t="s">
         <v>28</v>
@@ -4323,7 +4290,7 @@
         <v>45775</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="N7" s="8">
         <v>45792</v>
@@ -4332,10 +4299,10 @@
         <v>45775</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
@@ -4376,7 +4343,7 @@
         <v>45748</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="N8" s="8">
         <v>45792</v>
@@ -4385,10 +4352,10 @@
         <v>45691</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="102" x14ac:dyDescent="0.25">
@@ -4438,10 +4405,10 @@
         <v>45691</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -4517,7 +4484,7 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>35</v>
@@ -4526,25 +4493,25 @@
         <v>45779</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>25</v>
@@ -4553,7 +4520,7 @@
         <v>45779</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="N2" s="8">
         <v>45779</v>
@@ -4562,7 +4529,7 @@
         <v>45779</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="Q2" s="30" t="s">
         <v>28</v>
@@ -4668,7 +4635,7 @@
         <v>46164</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>25</v>
@@ -4677,7 +4644,7 @@
         <v>45761</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="N2" s="8">
         <v>45791</v>
@@ -4730,7 +4697,7 @@
         <v>45735</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="N3" s="8">
         <v>45761</v>
@@ -4783,7 +4750,7 @@
         <v>45722</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="N4" s="7">
         <v>45792</v>
@@ -4795,7 +4762,7 @@
         <v>49</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="293.25" x14ac:dyDescent="0.25">
@@ -4836,7 +4803,7 @@
         <v>45705</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="N5" s="11">
         <v>45792</v>
@@ -4848,7 +4815,7 @@
         <v>49</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
@@ -4889,7 +4856,7 @@
         <v>45708</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="N6" s="11">
         <v>45792</v>
@@ -4901,12 +4868,12 @@
         <v>49</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>35</v>
@@ -4915,7 +4882,7 @@
         <v>45791</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>148</v>
@@ -4924,7 +4891,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>39</v>
@@ -4933,7 +4900,7 @@
         <v>31</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>25</v>
@@ -4942,7 +4909,7 @@
         <v>45792</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="N7" s="11">
         <v>45792</v>
@@ -5143,7 +5110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I8" workbookViewId="0">
+    <sheetView topLeftCell="I8" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:Q10"/>
     </sheetView>
   </sheetViews>
@@ -5243,7 +5210,7 @@
         <v>45698</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="N2" s="7">
         <v>45793</v>
@@ -5296,7 +5263,7 @@
         <v>45744</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="N3" s="7">
         <v>45793</v>
@@ -5349,7 +5316,7 @@
         <v>45714</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="N4" s="7">
         <v>45793</v>
@@ -5402,7 +5369,7 @@
         <v>45734</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="N5" s="7">
         <v>45793</v>
@@ -5455,7 +5422,7 @@
         <v>45771</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="N6" s="7">
         <v>45793</v>
@@ -5508,7 +5475,7 @@
         <v>45748</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="N7" s="7">
         <v>45793</v>
@@ -5561,7 +5528,7 @@
         <v>45735</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="N8" s="7">
         <v>45793</v>
@@ -5614,7 +5581,7 @@
         <v>45769</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="N9" s="7">
         <v>45793</v>
@@ -5631,7 +5598,7 @@
     </row>
     <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>141</v>
@@ -5640,7 +5607,7 @@
         <v>45782</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>31</v>
@@ -5649,16 +5616,16 @@
         <v>31</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="I10" s="23" t="s">
         <v>31</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="K10" s="24" t="s">
         <v>25</v>
@@ -5667,7 +5634,7 @@
         <v>45792</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="N10" s="7">
         <v>45792</v>
@@ -5815,8 +5782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5915,7 +5882,7 @@
         <v>45735</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="N2" s="11">
         <v>45792</v>
@@ -5924,10 +5891,10 @@
         <v>45691</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
@@ -5968,7 +5935,7 @@
         <v>45712</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="N3" s="11">
         <v>45792</v>
@@ -5977,13 +5944,13 @@
         <v>45691</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q3" s="26" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="344.25" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>173</v>
       </c>
@@ -6012,81 +5979,81 @@
         <v>45466</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>178</v>
+        <v>296</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="8">
-        <v>45673</v>
+        <v>45748</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>179</v>
+        <v>297</v>
       </c>
       <c r="N4" s="7">
-        <v>45755</v>
+        <v>45783</v>
       </c>
       <c r="O4" s="8">
         <v>45691</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q4" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="27">
-        <v>45665</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="L5" s="27">
-        <v>45700</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="N5" s="7">
-        <v>45755</v>
+      <c r="C5" s="11">
+        <v>45684</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="11">
+        <v>46779</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="11">
+        <v>45735</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="N5" s="8">
+        <v>45792</v>
       </c>
       <c r="O5" s="8">
-        <v>45691</v>
+        <v>45688</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>28</v>
+        <v>178</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
@@ -6127,7 +6094,7 @@
         <v>45735</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="N6" s="8">
         <v>45792</v>
@@ -6136,10 +6103,10 @@
         <v>45688</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -6215,7 +6182,7 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>141</v>
@@ -6224,7 +6191,7 @@
         <v>36</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>31</v>
@@ -6233,16 +6200,16 @@
         <v>31</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>25</v>
@@ -6251,7 +6218,7 @@
         <v>36</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>123</v>
@@ -6260,7 +6227,7 @@
         <v>26</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>28</v>
@@ -6268,34 +6235,34 @@
     </row>
     <row r="3" spans="1:17" ht="382.5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="I3" s="11">
         <v>46395</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>25</v>
@@ -6304,7 +6271,7 @@
         <v>46</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>123</v>
@@ -6313,7 +6280,7 @@
         <v>27</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="Q3" s="9" t="s">
         <v>28</v>
@@ -6392,22 +6359,22 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C2" s="8">
         <v>43999</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>32</v>
@@ -6419,7 +6386,7 @@
         <v>44967</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>48</v>
@@ -6428,7 +6395,7 @@
         <v>45615</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="N2" s="8">
         <v>45791</v>
@@ -6437,7 +6404,7 @@
         <v>45691</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="Q2" s="15" t="s">
         <v>28</v>
@@ -6445,7 +6412,7 @@
     </row>
     <row r="3" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>18</v>
@@ -6454,7 +6421,7 @@
         <v>45266</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>31</v>
@@ -6472,7 +6439,7 @@
         <v>46232</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>25</v>
@@ -6481,7 +6448,7 @@
         <v>45693</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="N3" s="8">
         <v>45791</v>
@@ -6490,7 +6457,7 @@
         <v>45691</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>28</v>
@@ -6498,7 +6465,7 @@
     </row>
     <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>18</v>
@@ -6507,7 +6474,7 @@
         <v>44861</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>31</v>
@@ -6525,7 +6492,7 @@
         <v>45790</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>25</v>
@@ -6534,7 +6501,7 @@
         <v>45720</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="N4" s="8">
         <v>45761</v>
@@ -6543,7 +6510,7 @@
         <v>45691</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="Q4" s="15" t="s">
         <v>28</v>
@@ -6622,7 +6589,7 @@
     </row>
     <row r="2" spans="1:17" ht="229.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>18</v>
@@ -6631,25 +6598,25 @@
         <v>45700</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="I2" s="14">
         <v>46795</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>25</v>
@@ -6658,7 +6625,7 @@
         <v>45744</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="N2" s="8">
         <v>45777</v>
@@ -6667,7 +6634,7 @@
         <v>45701</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
actualizacion 19 de mayo final
</commit_message>
<xml_diff>
--- a/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
+++ b/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA EXPEDEDIENTES VIVOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DA1E72-7871-4E14-B660-E827DBEF5EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735D5C2F-3B55-4C8D-B2DC-38B144AB4D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSA" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="298">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -1816,8 +1816,8 @@
   </sheetPr>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O62" sqref="O62"/>
       <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
     </sheetView>
@@ -5780,10 +5780,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6053,59 +6053,6 @@
         <v>178</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="11">
-        <v>45684</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="11">
-        <v>46779</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="11">
-        <v>45735</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="N6" s="8">
-        <v>45792</v>
-      </c>
-      <c r="O6" s="8">
-        <v>45688</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q6" s="26" t="s">
         <v>276</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualizacion 19 de mayo shann
</commit_message>
<xml_diff>
--- a/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
+++ b/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA EXPEDEDIENTES VIVOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735D5C2F-3B55-4C8D-B2DC-38B144AB4D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD02EFF2-3235-4E25-AC8E-69247C16796B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <sheet name="SHANNERY CHAPARRO" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HSA!$A$1:$Q$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HSA!$A$1:$Q$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="298">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -893,9 +893,6 @@
     <t>REVOCATORIA DE MANDATO</t>
   </si>
   <si>
-    <t>02/05/2025 ASIGNADO A LA ASESORA SHANNERY CHAPARRO</t>
-  </si>
-  <si>
     <t>SHANNERY CHAPARRO</t>
   </si>
   <si>
@@ -1215,6 +1212,10 @@
 AUTO COMUNICADO EL 16 DE ENERO DE 2025, TÉRMINOS CUMPLIDOS EL 24 DE ENERO D 2025, EN PROYECCIÓN DECISIÓN
 16/01/2025 YA LLEGARON LAS NOTIFICACIONES
 15/01/2025 SE DEBE CORRER TRASLADO</t>
+  </si>
+  <si>
+    <t>14/05/2025 REALIZADA AUDIENCIA PÚBLICA
+02/05/2025 ASIGNADO A LA ASESORA SHANNERY CHAPARRO</t>
   </si>
 </sst>
 </file>
@@ -1814,12 +1815,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O62" sqref="O62"/>
-      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomLeft" activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1929,7 +1930,7 @@
         <v>46164</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>25</v>
@@ -1938,7 +1939,7 @@
         <v>45761</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N2" s="8">
         <v>45791</v>
@@ -1991,7 +1992,7 @@
         <v>45735</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N3" s="8">
         <v>45761</v>
@@ -2044,7 +2045,7 @@
         <v>45722</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N4" s="7">
         <v>45792</v>
@@ -2056,7 +2057,7 @@
         <v>49</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -2097,7 +2098,7 @@
         <v>45705</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N5" s="11">
         <v>45792</v>
@@ -2109,7 +2110,7 @@
         <v>49</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="127.5" x14ac:dyDescent="0.2">
@@ -2150,7 +2151,7 @@
         <v>45708</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N6" s="11">
         <v>45792</v>
@@ -2162,12 +2163,12 @@
         <v>49</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>35</v>
@@ -2176,7 +2177,7 @@
         <v>45791</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>148</v>
@@ -2185,7 +2186,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>39</v>
@@ -2194,7 +2195,7 @@
         <v>31</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>25</v>
@@ -2203,7 +2204,7 @@
         <v>45792</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N7" s="11">
         <v>45792</v>
@@ -2362,7 +2363,7 @@
         <v>45698</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N10" s="7">
         <v>45793</v>
@@ -2415,7 +2416,7 @@
         <v>45744</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N11" s="7">
         <v>45793</v>
@@ -2468,7 +2469,7 @@
         <v>45714</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N12" s="7">
         <v>45793</v>
@@ -2521,7 +2522,7 @@
         <v>45734</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N13" s="7">
         <v>45793</v>
@@ -2574,7 +2575,7 @@
         <v>45771</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N14" s="7">
         <v>45793</v>
@@ -2627,7 +2628,7 @@
         <v>45748</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N15" s="7">
         <v>45793</v>
@@ -2680,7 +2681,7 @@
         <v>45735</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N16" s="7">
         <v>45793</v>
@@ -2733,7 +2734,7 @@
         <v>45769</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N17" s="7">
         <v>45793</v>
@@ -2750,7 +2751,7 @@
     </row>
     <row r="18" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>141</v>
@@ -2759,16 +2760,16 @@
         <v>45782</v>
       </c>
       <c r="D18" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="22" t="s">
         <v>253</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>254</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>219</v>
@@ -2777,7 +2778,7 @@
         <v>31</v>
       </c>
       <c r="J18" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K18" s="24" t="s">
         <v>25</v>
@@ -2786,7 +2787,7 @@
         <v>45792</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N18" s="7">
         <v>45792</v>
@@ -2892,7 +2893,7 @@
         <v>45735</v>
       </c>
       <c r="M20" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N20" s="11">
         <v>45792</v>
@@ -2904,7 +2905,7 @@
         <v>178</v>
       </c>
       <c r="Q20" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="140.25" x14ac:dyDescent="0.2">
@@ -2945,7 +2946,7 @@
         <v>45712</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N21" s="11">
         <v>45792</v>
@@ -2957,7 +2958,7 @@
         <v>178</v>
       </c>
       <c r="Q21" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
@@ -2989,7 +2990,7 @@
         <v>45466</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K22" s="15" t="s">
         <v>25</v>
@@ -2998,7 +2999,7 @@
         <v>45748</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N22" s="7">
         <v>45783</v>
@@ -3051,7 +3052,7 @@
         <v>45735</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N23" s="8">
         <v>45792</v>
@@ -3063,7 +3064,7 @@
         <v>178</v>
       </c>
       <c r="Q23" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -3210,7 +3211,7 @@
         <v>45615</v>
       </c>
       <c r="M26" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N26" s="8">
         <v>45791</v>
@@ -3263,7 +3264,7 @@
         <v>45693</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N27" s="8">
         <v>45791</v>
@@ -3316,7 +3317,7 @@
         <v>45720</v>
       </c>
       <c r="M28" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N28" s="8">
         <v>45761</v>
@@ -3413,7 +3414,7 @@
         <v>46992</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>25</v>
@@ -3422,7 +3423,7 @@
         <v>45784</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N30" s="8">
         <v>45793</v>
@@ -3475,7 +3476,7 @@
         <v>45735</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N31" s="8">
         <v>45761</v>
@@ -3492,7 +3493,7 @@
     </row>
     <row r="32" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>35</v>
@@ -3501,25 +3502,25 @@
         <v>45417</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>30</v>
       </c>
       <c r="F32" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="G32" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="H32" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="H32" s="9" t="s">
-        <v>251</v>
-      </c>
       <c r="I32" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>25</v>
@@ -3528,7 +3529,7 @@
         <v>45786</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N32" s="8">
         <v>45791</v>
@@ -3572,7 +3573,7 @@
         <v>31</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K33" s="9" t="s">
         <v>25</v>
@@ -3581,7 +3582,7 @@
         <v>45786</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N33" s="11">
         <v>45791</v>
@@ -3634,7 +3635,7 @@
         <v>45775</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N34" s="8">
         <v>45792</v>
@@ -3646,7 +3647,7 @@
         <v>213</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="165.75" x14ac:dyDescent="0.2">
@@ -3687,7 +3688,7 @@
         <v>45748</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N35" s="8">
         <v>45792</v>
@@ -3699,7 +3700,7 @@
         <v>213</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
@@ -3752,7 +3753,7 @@
         <v>213</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
@@ -3837,85 +3838,32 @@
         <v>31</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>245</v>
+        <v>297</v>
       </c>
       <c r="K38" s="13" t="s">
         <v>25</v>
       </c>
       <c r="L38" s="14">
-        <v>45779</v>
+        <v>45791</v>
       </c>
       <c r="M38" s="13" t="s">
-        <v>245</v>
+        <v>297</v>
       </c>
       <c r="N38" s="8">
         <v>45779</v>
       </c>
       <c r="O38" s="14">
-        <v>45779</v>
+        <v>45791</v>
       </c>
       <c r="P38" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q38" s="30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="14">
-        <v>45779</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L39" s="14">
-        <v>45779</v>
-      </c>
-      <c r="M39" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="N39" s="8">
-        <v>45779</v>
-      </c>
-      <c r="O39" s="14">
-        <v>45779</v>
-      </c>
-      <c r="P39" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="Q39" s="30" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:Q39" xr:uid="{868CBA12-E8F6-468A-9E1A-12215A2C5AF4}"/>
+  <autoFilter ref="A1:Q38" xr:uid="{868CBA12-E8F6-468A-9E1A-12215A2C5AF4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -4069,7 +4017,7 @@
         <v>46992</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>25</v>
@@ -4078,7 +4026,7 @@
         <v>45784</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N3" s="8">
         <v>45793</v>
@@ -4131,7 +4079,7 @@
         <v>45735</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N4" s="8">
         <v>45761</v>
@@ -4148,7 +4096,7 @@
     </row>
     <row r="5" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>35</v>
@@ -4157,25 +4105,25 @@
         <v>45417</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>30</v>
       </c>
       <c r="F5" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="G5" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="H5" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>251</v>
-      </c>
       <c r="I5" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>25</v>
@@ -4184,7 +4132,7 @@
         <v>45786</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N5" s="8">
         <v>45791</v>
@@ -4228,7 +4176,7 @@
         <v>31</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>25</v>
@@ -4237,7 +4185,7 @@
         <v>45786</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N6" s="11">
         <v>45791</v>
@@ -4290,7 +4238,7 @@
         <v>45775</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N7" s="8">
         <v>45792</v>
@@ -4302,7 +4250,7 @@
         <v>213</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
@@ -4343,7 +4291,7 @@
         <v>45748</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N8" s="8">
         <v>45792</v>
@@ -4355,7 +4303,7 @@
         <v>213</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="102" x14ac:dyDescent="0.25">
@@ -4408,7 +4356,7 @@
         <v>213</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -4421,7 +4369,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4511,25 +4459,25 @@
         <v>31</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>245</v>
+        <v>297</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>25</v>
       </c>
       <c r="L2" s="14">
-        <v>45779</v>
+        <v>45791</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>245</v>
+        <v>297</v>
       </c>
       <c r="N2" s="8">
-        <v>45779</v>
+        <v>45791</v>
       </c>
       <c r="O2" s="14">
         <v>45779</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q2" s="30" t="s">
         <v>28</v>
@@ -4635,7 +4583,7 @@
         <v>46164</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>25</v>
@@ -4644,7 +4592,7 @@
         <v>45761</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N2" s="8">
         <v>45791</v>
@@ -4697,7 +4645,7 @@
         <v>45735</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N3" s="8">
         <v>45761</v>
@@ -4750,7 +4698,7 @@
         <v>45722</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N4" s="7">
         <v>45792</v>
@@ -4762,7 +4710,7 @@
         <v>49</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="293.25" x14ac:dyDescent="0.25">
@@ -4803,7 +4751,7 @@
         <v>45705</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N5" s="11">
         <v>45792</v>
@@ -4815,7 +4763,7 @@
         <v>49</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
@@ -4856,7 +4804,7 @@
         <v>45708</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N6" s="11">
         <v>45792</v>
@@ -4868,12 +4816,12 @@
         <v>49</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>35</v>
@@ -4882,7 +4830,7 @@
         <v>45791</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>148</v>
@@ -4891,7 +4839,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>39</v>
@@ -4900,7 +4848,7 @@
         <v>31</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>25</v>
@@ -4909,7 +4857,7 @@
         <v>45792</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N7" s="11">
         <v>45792</v>
@@ -5210,7 +5158,7 @@
         <v>45698</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N2" s="7">
         <v>45793</v>
@@ -5263,7 +5211,7 @@
         <v>45744</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N3" s="7">
         <v>45793</v>
@@ -5316,7 +5264,7 @@
         <v>45714</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N4" s="7">
         <v>45793</v>
@@ -5369,7 +5317,7 @@
         <v>45734</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N5" s="7">
         <v>45793</v>
@@ -5422,7 +5370,7 @@
         <v>45771</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N6" s="7">
         <v>45793</v>
@@ -5475,7 +5423,7 @@
         <v>45748</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N7" s="7">
         <v>45793</v>
@@ -5528,7 +5476,7 @@
         <v>45735</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N8" s="7">
         <v>45793</v>
@@ -5581,7 +5529,7 @@
         <v>45769</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N9" s="7">
         <v>45793</v>
@@ -5598,7 +5546,7 @@
     </row>
     <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>141</v>
@@ -5607,16 +5555,16 @@
         <v>45782</v>
       </c>
       <c r="D10" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="22" t="s">
         <v>253</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>254</v>
       </c>
       <c r="H10" s="22" t="s">
         <v>219</v>
@@ -5625,7 +5573,7 @@
         <v>31</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K10" s="24" t="s">
         <v>25</v>
@@ -5634,7 +5582,7 @@
         <v>45792</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N10" s="7">
         <v>45792</v>
@@ -5882,7 +5830,7 @@
         <v>45735</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N2" s="11">
         <v>45792</v>
@@ -5894,7 +5842,7 @@
         <v>178</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
@@ -5935,7 +5883,7 @@
         <v>45712</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N3" s="11">
         <v>45792</v>
@@ -5947,7 +5895,7 @@
         <v>178</v>
       </c>
       <c r="Q3" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
@@ -5979,7 +5927,7 @@
         <v>45466</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>25</v>
@@ -5988,7 +5936,7 @@
         <v>45748</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N4" s="7">
         <v>45783</v>
@@ -6041,7 +5989,7 @@
         <v>45735</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N5" s="8">
         <v>45792</v>
@@ -6053,7 +6001,7 @@
         <v>178</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -6342,7 +6290,7 @@
         <v>45615</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N2" s="8">
         <v>45791</v>
@@ -6395,7 +6343,7 @@
         <v>45693</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N3" s="8">
         <v>45791</v>
@@ -6448,7 +6396,7 @@
         <v>45720</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N4" s="8">
         <v>45761</v>

</xml_diff>

<commit_message>
actualizacion 27 de mayo
</commit_message>
<xml_diff>
--- a/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
+++ b/HSA H.M ALVARO ECHEVERRY EXPEDIENTES ACTIVOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA EXPEDEDIENTES VIVOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D193722-2578-471D-BE1A-57D5C91B7D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDF941-051A-44AB-BAB1-6BE52D1102C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSA" sheetId="11" r:id="rId1"/>
@@ -1657,7 +1657,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{2AF8BEAA-C327-4F20-8D05-10D15FA1704F}"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2157,8 +2171,8 @@
   </sheetPr>
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O62" sqref="O62"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:Q44"/>
     </sheetView>
@@ -2900,7 +2914,7 @@
         <v>114</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="I14" s="7">
         <v>46145</v>
@@ -3217,7 +3231,7 @@
       <c r="G20" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="9" t="s">
         <v>300</v>
       </c>
       <c r="I20" s="23" t="s">
@@ -3376,8 +3390,8 @@
       <c r="G23" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="H23" s="26" t="s">
-        <v>159</v>
+      <c r="H23" s="22" t="s">
+        <v>138</v>
       </c>
       <c r="I23" s="25">
         <v>46315</v>
@@ -3641,8 +3655,8 @@
       <c r="G28" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="H28" s="15" t="s">
-        <v>191</v>
+      <c r="H28" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="I28" s="8">
         <v>46395</v>
@@ -3694,8 +3708,8 @@
       <c r="G29" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="H29" s="15" t="s">
-        <v>317</v>
+      <c r="H29" s="9" t="s">
+        <v>300</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>31</v>
@@ -3906,7 +3920,7 @@
       <c r="G33" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="22" t="s">
         <v>219</v>
       </c>
       <c r="I33" s="7">
@@ -4171,7 +4185,7 @@
       <c r="G38" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="H38" s="6" t="s">
         <v>39</v>
       </c>
       <c r="I38" s="11" t="s">
@@ -4436,8 +4450,8 @@
       <c r="G43" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="H43" s="13" t="s">
-        <v>210</v>
+      <c r="H43" s="22" t="s">
+        <v>219</v>
       </c>
       <c r="I43" s="14">
         <v>46795</v>
@@ -4522,70 +4536,54 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Q38" xr:uid="{868CBA12-E8F6-468A-9E1A-12215A2C5AF4}"/>
-  <conditionalFormatting sqref="M44">
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="M8">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="14">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M42">
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="greaterThan">
+  <conditionalFormatting sqref="M20:M21">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="12">
-      <formula>"m2&gt;60"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M21">
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="greaterThan">
-      <formula>60</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="10">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="M41:M42">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M41">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="M44">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="4">
-      <formula>"m2&gt;60"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M20">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
-      <formula>60</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A44" r:id="rId1" xr:uid="{EAAD91A2-90E6-4380-9C68-67BDD3DA4475}"/>
-    <hyperlink ref="A42" r:id="rId2" xr:uid="{311DD614-99E6-40A8-B118-7F3F072A87A3}"/>
-    <hyperlink ref="A21" r:id="rId3" xr:uid="{9738EE7E-A813-4039-8B1F-A6E05CCA84C2}"/>
-    <hyperlink ref="A29" r:id="rId4" xr:uid="{984D0010-BD3F-4E1D-B2DC-DBE8615E186A}"/>
-    <hyperlink ref="A8" r:id="rId5" xr:uid="{98008150-9209-4FD2-A563-B2A96339AFFE}"/>
-    <hyperlink ref="A41" r:id="rId6" xr:uid="{B56A2A39-D410-4952-AAFF-8276E6F40980}"/>
-    <hyperlink ref="A20" r:id="rId7" xr:uid="{4D5A7938-F9CE-4B42-AD08-B74E312AE320}"/>
+    <hyperlink ref="A44" r:id="rId1" xr:uid="{0809FA27-3576-40C9-AEAE-BCC9B25E8DE6}"/>
+    <hyperlink ref="A42" r:id="rId2" xr:uid="{CAC71FA8-B4D8-4906-BE90-68157FCDA747}"/>
+    <hyperlink ref="A21" r:id="rId3" xr:uid="{CFE81EA7-7FA8-4851-A85C-DD06B7825F9F}"/>
+    <hyperlink ref="A29" r:id="rId4" xr:uid="{B53542DA-E187-40BE-8A7C-CCDD9124C4D5}"/>
+    <hyperlink ref="A8" r:id="rId5" xr:uid="{67E7F4AB-8E3B-473A-8362-3C2CF81EE24E}"/>
+    <hyperlink ref="A41" r:id="rId6" xr:uid="{78C9E305-76D0-4D34-95FF-FB8EC5A41BA3}"/>
+    <hyperlink ref="A20" r:id="rId7" xr:uid="{E2EC3D5A-6E3B-47F5-9A98-2D927CB8241D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -5189,19 +5187,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="M10:M11">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>"m2&gt;60"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
-      <formula>60</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5217,7 +5207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A65B1D2-9DDC-4748-A89D-A3B554A960BE}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -5355,10 +5345,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5808,10 +5798,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6865,19 +6855,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="U11">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="U11:U12">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
-      <formula>"m2&gt;60"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U12">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
-      <formula>60</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7523,10 +7505,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M4">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>